<commit_message>
update excel file 30.11.24
</commit_message>
<xml_diff>
--- a/URS_Certifications 30.11.24.xlsx
+++ b/URS_Certifications 30.11.24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\сайт\сайт2\Сайт на практику\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED39CA9A-ECAB-41AB-89E9-3667DD90831F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7D97EF-3855-4179-9AAA-EEE766F94D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URS_Certifications 30.11.24" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5861" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5860" uniqueCount="731">
   <si>
     <t>Название компании</t>
   </si>
@@ -3075,8 +3075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A616" workbookViewId="0">
-      <selection activeCell="I629" sqref="I629"/>
+    <sheetView tabSelected="1" topLeftCell="A1181" workbookViewId="0">
+      <selection activeCell="I1188" sqref="I1188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26989,9 +26989,6 @@
       <c r="E1195" t="s">
         <v>604</v>
       </c>
-      <c r="F1195" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="1196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1196" t="s">

</xml_diff>